<commit_message>
criado novo para gerar os mapas de rastros a partir de um csv feito pelo arquivo de processamento de colhedoras
</commit_message>
<xml_diff>
--- a/dados/cav ouroeste.xlsx
+++ b/dados/cav ouroeste.xlsx
@@ -97,10 +97,10 @@
     <t>485699</t>
   </si>
   <si>
-    <t>10/06/2025 00:00</t>
-  </si>
-  <si>
-    <t>10/06/2025 23:59</t>
+    <t>11/06/2025 00:00</t>
+  </si>
+  <si>
+    <t>11/06/2025 23:59</t>
   </si>
   <si>
     <t>6126</t>
@@ -682,46 +682,46 @@
         <v>29</v>
       </c>
       <c r="I2">
-        <v>22.099999999999454</v>
+        <v>19.400000000000546</v>
       </c>
       <c r="J2">
-        <v>8067.95</v>
+        <v>8088.7</v>
       </c>
       <c r="K2">
-        <v>38.08299416666668</v>
+        <v>63.75316611111114</v>
       </c>
       <c r="L2">
-        <v>160.34236277777782</v>
+        <v>225.91780083333344</v>
       </c>
       <c r="M2">
-        <v>8.091688888888887</v>
+        <v>3.4775955555555553</v>
       </c>
       <c r="N2">
-        <v>6.813266825801988</v>
+        <v>6.652043398232149</v>
       </c>
       <c r="O2">
-        <v>21.887358821544616</v>
+        <v>20.35943581424459</v>
       </c>
       <c r="P2">
-        <v>29.699017271333677</v>
+        <v>35.10527265077139</v>
       </c>
       <c r="Q2">
-        <v>206.51704277777785</v>
+        <v>293.1485652777778</v>
       </c>
       <c r="R2">
-        <v>681.4051487935111</v>
+        <v>967.2467659565131</v>
       </c>
       <c r="S2">
-        <v>0.428</v>
+        <v>0.68</v>
       </c>
       <c r="T2">
-        <v>15.693423054560068</v>
+        <v>14.123999431917145</v>
       </c>
       <c r="U2">
-        <v>51.780613976149276</v>
+        <v>46.60228427162318</v>
       </c>
       <c r="V2">
-        <v>0.2836840895997529</v>
+        <v>0.27723785433317394</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -779,46 +779,46 @@
         <v>29</v>
       </c>
       <c r="I4">
-        <v>26.100000000000364</v>
+        <v>19.350000000000364</v>
       </c>
       <c r="J4">
-        <v>8104.6</v>
+        <v>8121.9</v>
       </c>
       <c r="K4">
-        <v>41.98930722222222</v>
+        <v>42.92891833333333</v>
       </c>
       <c r="L4">
-        <v>270.43471722222216</v>
+        <v>231.72235194444448</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>5.187343857890824</v>
+        <v>4.853603143051577</v>
       </c>
       <c r="O4">
-        <v>23.604816609650893</v>
+        <v>19.497712057964243</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>312.4240305555555</v>
+        <v>274.6512716666666</v>
       </c>
       <c r="R4">
-        <v>1030.8463658200533</v>
+        <v>906.2147516693477</v>
       </c>
       <c r="S4">
-        <v>0.48</v>
+        <v>0.3</v>
       </c>
       <c r="T4">
-        <v>16.01147379932575</v>
+        <v>13.277337253372947</v>
       </c>
       <c r="U4">
-        <v>52.830025744524</v>
+        <v>43.80871353291403</v>
       </c>
       <c r="V4">
-        <v>0.27433176728648584</v>
+        <v>0.2752595992742738</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -905,46 +905,46 @@
         <v>29</v>
       </c>
       <c r="I7">
-        <v>28.950000000000728</v>
+        <v>20.400000000001455</v>
       </c>
       <c r="J7">
-        <v>8318.35</v>
+        <v>8338.45</v>
       </c>
       <c r="K7">
-        <v>49.94443611111111</v>
+        <v>67.70883583333332</v>
       </c>
       <c r="L7">
-        <v>247.78090472222217</v>
+        <v>181.30918999999994</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>0.02260527777777778</v>
       </c>
       <c r="N7">
-        <v>5.6371531034221105</v>
+        <v>5.975965089363547</v>
       </c>
       <c r="O7">
-        <v>20.86985554526143</v>
+        <v>17.840973894813946</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>38.269</v>
       </c>
       <c r="Q7">
-        <v>297.72534222222225</v>
+        <v>249.04063527777774</v>
       </c>
       <c r="R7">
-        <v>982.3478894903209</v>
+        <v>821.7121882753635</v>
       </c>
       <c r="S7">
-        <v>0.5479999999999999</v>
+        <v>0.608</v>
       </c>
       <c r="T7">
-        <v>14.391723227971664</v>
+        <v>11.600214124440885</v>
       </c>
       <c r="U7">
-        <v>47.485641744848266</v>
+        <v>38.275028177731514</v>
       </c>
       <c r="V7">
-        <v>0.2796326882820518</v>
+        <v>0.2839910145897543</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -973,46 +973,46 @@
         <v>29</v>
       </c>
       <c r="I8">
-        <v>31.099999999999454</v>
+        <v>21.25</v>
       </c>
       <c r="J8">
-        <v>6330.9</v>
+        <v>6348.7</v>
       </c>
       <c r="K8">
-        <v>51.866613055555554</v>
+        <v>55.304571666666654</v>
       </c>
       <c r="L8">
-        <v>234.3464075</v>
+        <v>193.68677277777772</v>
       </c>
       <c r="M8">
-        <v>4.693389999999999</v>
+        <v>0.5724213888888889</v>
       </c>
       <c r="N8">
-        <v>4.7986444708400775</v>
+        <v>4.950021491339216</v>
       </c>
       <c r="O8">
-        <v>19.594238882295976</v>
+        <v>18.10333113347889</v>
       </c>
       <c r="P8">
-        <v>29.76202223791034</v>
+        <v>27.117877146631436</v>
       </c>
       <c r="Q8">
-        <v>290.9064147222222</v>
+        <v>249.56376138888902</v>
       </c>
       <c r="R8">
-        <v>959.8487666806384</v>
+        <v>823.4382483660221</v>
       </c>
       <c r="S8">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="T8">
-        <v>12.747174060779447</v>
+        <v>11.495198867374963</v>
       </c>
       <c r="U8">
-        <v>42.05943451809323</v>
+        <v>37.928529235542065</v>
       </c>
       <c r="V8">
-        <v>0.27142232704717734</v>
+        <v>0.27292770816897716</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1070,46 +1070,46 @@
         <v>29</v>
       </c>
       <c r="I10">
-        <v>21.600000000000364</v>
+        <v>17.850000000000364</v>
       </c>
       <c r="J10">
-        <v>8807.95</v>
+        <v>8828.95</v>
       </c>
       <c r="K10">
-        <v>31.453763055555562</v>
+        <v>45.80332444444445</v>
       </c>
       <c r="L10">
-        <v>158.73907111111114</v>
+        <v>149.89100833333333</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>0.08514583333333332</v>
       </c>
       <c r="N10">
-        <v>5.260971175061982</v>
+        <v>4.738515685037058</v>
       </c>
       <c r="O10">
-        <v>17.322623269109517</v>
+        <v>17.11427156123925</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>20.291</v>
       </c>
       <c r="Q10">
-        <v>190.19283277777774</v>
+        <v>195.77948083333334</v>
       </c>
       <c r="R10">
-        <v>627.5432466745858</v>
+        <v>645.9764505319987</v>
       </c>
       <c r="S10">
-        <v>0.58</v>
+        <v>0.7</v>
       </c>
       <c r="T10">
-        <v>12.596300969495639</v>
+        <v>10.688962707586514</v>
       </c>
       <c r="U10">
-        <v>41.56162717090104</v>
+        <v>35.268344569744244</v>
       </c>
       <c r="V10">
-        <v>0.2791726863843192</v>
+        <v>0.2610135727322735</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1167,46 +1167,46 @@
         <v>29</v>
       </c>
       <c r="I12">
-        <v>23</v>
+        <v>18.25</v>
       </c>
       <c r="J12">
-        <v>900.8</v>
+        <v>920.75</v>
       </c>
       <c r="K12">
-        <v>73.7509541666667</v>
+        <v>95.89975750000005</v>
       </c>
       <c r="L12">
-        <v>140.68745083333332</v>
+        <v>177.95285222222222</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>0.3321738888888889</v>
       </c>
       <c r="N12">
-        <v>9.234595077708489</v>
+        <v>10.240484505078964</v>
       </c>
       <c r="O12">
-        <v>16.024560149329282</v>
+        <v>18.650448700669237</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>25.156421276595744</v>
       </c>
       <c r="Q12">
-        <v>214.43840416666652</v>
+        <v>274.1847836111112</v>
       </c>
       <c r="R12">
-        <v>707.5417637829627</v>
+        <v>904.6755694370698</v>
       </c>
       <c r="S12">
-        <v>0.5479999999999999</v>
+        <v>0.496</v>
       </c>
       <c r="T12">
-        <v>12.79000239551115</v>
+        <v>14.492057236981184</v>
       </c>
       <c r="U12">
-        <v>42.200747057765014</v>
+        <v>47.81669485997421</v>
       </c>
       <c r="V12">
-        <v>0.3587037576890657</v>
+        <v>0.3580057076203627</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -1235,46 +1235,46 @@
         <v>29</v>
       </c>
       <c r="I13">
-        <v>27.049999999999955</v>
+        <v>20.299999999999955</v>
       </c>
       <c r="J13">
-        <v>898.15</v>
+        <v>919.35</v>
       </c>
       <c r="K13">
-        <v>56.43683055555556</v>
+        <v>65.34161027777778</v>
       </c>
       <c r="L13">
-        <v>171.21410388888887</v>
+        <v>222.7585213888889</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>0.10196666666666666</v>
       </c>
       <c r="N13">
-        <v>6.400519968124077</v>
+        <v>7.432575328876699</v>
       </c>
       <c r="O13">
-        <v>15.967152238558535</v>
+        <v>19.3091795331099</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>22.215</v>
       </c>
       <c r="Q13">
-        <v>227.65093499999995</v>
+        <v>288.20209694444446</v>
       </c>
       <c r="R13">
-        <v>751.1366478532045</v>
+        <v>950.9258418073897</v>
       </c>
       <c r="S13">
-        <v>0.41200000000000003</v>
+        <v>0.428</v>
       </c>
       <c r="T13">
-        <v>11.650080573334868</v>
+        <v>14.174492627431912</v>
       </c>
       <c r="U13">
-        <v>38.43956304890421</v>
+        <v>46.76888709984508</v>
       </c>
       <c r="V13">
-        <v>0.32217157199166185</v>
+        <v>0.32642344539726603</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1448,46 +1448,46 @@
         <v>29</v>
       </c>
       <c r="I19">
-        <v>10.050000000000068</v>
+        <v>16.5</v>
       </c>
       <c r="J19">
-        <v>912.7</v>
+        <v>928.65</v>
       </c>
       <c r="K19">
-        <v>22.555659444444448</v>
+        <v>93.16018305555555</v>
       </c>
       <c r="L19">
-        <v>54.21273138888888</v>
+        <v>190.67577916666676</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>4.571635</v>
       </c>
       <c r="N19">
-        <v>9.819199187483376</v>
+        <v>10.454452363439158</v>
       </c>
       <c r="O19">
-        <v>23.93152100345766</v>
+        <v>23.64379718820174</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>31.25084423735261</v>
       </c>
       <c r="Q19">
-        <v>76.76839194444445</v>
+        <v>288.4075988888889</v>
       </c>
       <c r="R19">
-        <v>253.2981144410014</v>
+        <v>951.6038976285851</v>
       </c>
       <c r="S19">
-        <v>0.784</v>
+        <v>0.49200000000000005</v>
       </c>
       <c r="T19">
-        <v>16.825868059952267</v>
+        <v>16.84425112417512</v>
       </c>
       <c r="U19">
-        <v>55.51712814960699</v>
+        <v>55.57778326282945</v>
       </c>
       <c r="V19">
-        <v>0.40420262062628465</v>
+        <v>0.38509395188315826</v>
       </c>
     </row>
   </sheetData>

</xml_diff>